<commit_message>
Update 7/16/2019 with summaries in notes sections
</commit_message>
<xml_diff>
--- a/Students_test/farmers-spf231.xlsx
+++ b/Students_test/farmers-spf231.xlsx
@@ -11,12 +11,12 @@
   <definedNames>
     <definedName localSheetId="0" name="_xlnm.Print_Area">'PPF 2007'!$A$1:$M$114</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="151">
   <si>
     <t>BIOLOGICAL ENGINEERING</t>
   </si>
@@ -192,12 +192,18 @@
     <t>Biochemistry</t>
   </si>
   <si>
+    <t>BIOMG3300</t>
+  </si>
+  <si>
     <t xml:space="preserve">    BIOMG 3300 (4) or 3330 (4) or 3310+3320 (5) or 3350 (4)</t>
   </si>
   <si>
     <t>Advanced Biol. Sci. Elective (to complete 15 cr)</t>
   </si>
   <si>
+    <t>BIONB2220</t>
+  </si>
+  <si>
     <t>5.</t>
   </si>
   <si>
@@ -391,6 +397,78 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>The following courses are needed for graduation:</t>
+  </si>
+  <si>
+    <t>MATH1920</t>
+  </si>
+  <si>
+    <t>MATH2930</t>
+  </si>
+  <si>
+    <t>MATH2940</t>
+  </si>
+  <si>
+    <t>PHYS1112</t>
+  </si>
+  <si>
+    <t>PHYS2213</t>
+  </si>
+  <si>
+    <t>CHEM2070 or CHEM2090</t>
+  </si>
+  <si>
+    <t>Intro Bio(6 credits)</t>
+  </si>
+  <si>
+    <t>BIOG1500 or BIOSM1500</t>
+  </si>
+  <si>
+    <t>Biochemistry(4 credits)</t>
+  </si>
+  <si>
+    <t>Advanced Biology to complete 15 credits of Biological Sciences</t>
+  </si>
+  <si>
+    <t>FWS(6 credits)</t>
+  </si>
+  <si>
+    <t>Liberal Arts(18 credits)</t>
+  </si>
+  <si>
+    <t>BEE1510 or CS1112</t>
+  </si>
+  <si>
+    <t>ENGRD2020</t>
+  </si>
+  <si>
+    <t>CEE3040 or ENGRD2700</t>
+  </si>
+  <si>
+    <t>BEE1200</t>
+  </si>
+  <si>
+    <t>BEE2600 or BEE2510</t>
+  </si>
+  <si>
+    <t>BEE3310</t>
+  </si>
+  <si>
+    <t>BEE3400</t>
+  </si>
+  <si>
+    <t>BEE3500</t>
+  </si>
+  <si>
+    <t>BEE3600</t>
+  </si>
+  <si>
+    <t>BEE4500</t>
+  </si>
+  <si>
+    <t>Focus Areas to complete 48 credits of Engineering Requirements</t>
   </si>
 </sst>
 </file>
@@ -451,6 +529,7 @@
     </font>
     <font>
       <name val="Monaco"/>
+      <family val="2"/>
       <sz val="9"/>
     </font>
   </fonts>
@@ -547,11 +626,47 @@
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
@@ -575,50 +690,14 @@
     <xf applyAlignment="1" borderId="3" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -952,43 +1031,43 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N111"/>
+  <dimension ref="A1:N135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0" zoomScale="80" zoomScaleNormal="80">
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0" zoomScale="80" zoomScaleNormal="80">
       <selection activeCell="I84" sqref="I84:K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="7.5"/>
-    <col customWidth="1" max="3" min="2" style="31" width="9.1640625"/>
-    <col customWidth="1" max="4" min="4" style="31" width="6.33203125"/>
-    <col customWidth="1" max="5" min="5" style="31" width="9.5"/>
-    <col customWidth="1" max="6" min="6" style="31" width="2.5"/>
-    <col customWidth="1" max="7" min="7" style="31" width="9.1640625"/>
-    <col customWidth="1" max="8" min="8" style="31" width="19.5"/>
-    <col customWidth="1" max="9" min="9" style="31" width="9.5"/>
-    <col customWidth="1" max="10" min="10" style="31" width="1.6640625"/>
-    <col customWidth="1" max="11" min="11" style="31" width="9.5"/>
-    <col customWidth="1" max="12" min="12" style="31" width="5.1640625"/>
-    <col customWidth="1" max="13" min="13" style="31" width="9.6640625"/>
-    <col customWidth="1" max="17" min="14" style="31" width="9.1640625"/>
-    <col customWidth="1" max="16384" min="18" style="31" width="9.1640625"/>
+    <col customWidth="1" max="3" min="2" style="32" width="9.1640625"/>
+    <col customWidth="1" max="4" min="4" style="32" width="6.33203125"/>
+    <col customWidth="1" max="5" min="5" style="32" width="9.5"/>
+    <col customWidth="1" max="6" min="6" style="32" width="2.5"/>
+    <col customWidth="1" max="7" min="7" style="32" width="9.1640625"/>
+    <col customWidth="1" max="8" min="8" style="32" width="19.5"/>
+    <col customWidth="1" max="9" min="9" style="32" width="9.5"/>
+    <col customWidth="1" max="10" min="10" style="32" width="1.6640625"/>
+    <col customWidth="1" max="11" min="11" style="32" width="9.5"/>
+    <col customWidth="1" max="12" min="12" style="32" width="5.1640625"/>
+    <col customWidth="1" max="13" min="13" style="32" width="9.6640625"/>
+    <col customWidth="1" max="18" min="14" style="32" width="9.1640625"/>
+    <col customWidth="1" max="16384" min="19" style="32" width="9.1640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="5" t="n"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="31" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
     </row>
@@ -996,41 +1075,41 @@
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="45" t="n">
+      <c r="L5" s="33" t="n">
         <v>43505</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="33" t="n">
+      <c r="G6" s="37" t="n">
         <v>3055888</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="31" t="n"/>
+      <c r="L6" s="32" t="n"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="31" t="n"/>
-      <c r="F7" s="31" t="n"/>
-      <c r="J7" s="38" t="s">
+      <c r="B7" s="32" t="n"/>
+      <c r="F7" s="32" t="n"/>
+      <c r="J7" s="34" t="s">
         <v>11</v>
       </c>
       <c r="M7" s="7" t="s">
@@ -1041,7 +1120,7 @@
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="48" t="n"/>
+      <c r="B8" s="38" t="n"/>
       <c r="J8" s="11" t="s">
         <v>14</v>
       </c>
@@ -1049,45 +1128,45 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2" t="n"/>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="16" t="n"/>
       <c r="E9" s="16" t="n"/>
       <c r="F9" s="16" t="n"/>
-      <c r="G9" s="42" t="n"/>
+      <c r="G9" s="40" t="n"/>
       <c r="H9" s="16" t="n"/>
-      <c r="I9" s="42" t="n"/>
+      <c r="I9" s="40" t="n"/>
       <c r="J9" s="16" t="n"/>
-      <c r="K9" s="42" t="s">
+      <c r="K9" s="40" t="s">
         <v>16</v>
       </c>
       <c r="L9" s="16" t="n"/>
-      <c r="M9" s="42" t="s">
+      <c r="M9" s="40" t="s">
         <v>17</v>
       </c>
     </row>
     <row customHeight="1" ht="14" r="10" spans="1:14" thickBot="1">
       <c r="A10" s="3" t="n"/>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="48" t="n"/>
-      <c r="E10" s="48" t="n"/>
-      <c r="F10" s="48" t="n"/>
-      <c r="G10" s="43" t="s">
+      <c r="D10" s="38" t="n"/>
+      <c r="E10" s="38" t="n"/>
+      <c r="F10" s="38" t="n"/>
+      <c r="G10" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="43" t="n"/>
-      <c r="I10" s="43" t="s">
+      <c r="H10" s="41" t="n"/>
+      <c r="I10" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="48" t="n"/>
-      <c r="K10" s="43" t="s">
+      <c r="J10" s="38" t="n"/>
+      <c r="K10" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="48" t="n"/>
-      <c r="M10" s="43" t="s">
+      <c r="L10" s="38" t="n"/>
+      <c r="M10" s="41" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1095,76 +1174,76 @@
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="35" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="4" t="n"/>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="35" t="s">
+      <c r="I12" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="35" t="n">
+      <c r="K12" s="44" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="4" t="n"/>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="36" t="s">
+      <c r="I13" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="35" t="s">
+      <c r="K13" s="44" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="4" t="n"/>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="36" t="s">
+      <c r="I14" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="35" t="s">
+      <c r="K14" s="44" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="4" t="n"/>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="36" t="s">
+      <c r="I15" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="35" t="s">
+      <c r="K15" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="M15" s="35" t="n">
+      <c r="M15" s="44" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="4" t="n"/>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="32" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1175,44 +1254,44 @@
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="34" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="4" t="n"/>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="I19" s="35" t="n"/>
-      <c r="K19" s="35" t="n"/>
+      <c r="I19" s="44" t="n"/>
+      <c r="K19" s="44" t="n"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="4" t="n"/>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="35" t="n"/>
-      <c r="K20" s="36" t="n"/>
-      <c r="M20" s="35" t="n">
+      <c r="I20" s="44" t="n"/>
+      <c r="K20" s="48" t="n"/>
+      <c r="M20" s="44" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="4" t="n"/>
-      <c r="G21" s="38" t="n"/>
+      <c r="G21" s="34" t="n"/>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="34" t="s">
         <v>44</v>
       </c>
       <c r="I22" s="10" t="n"/>
@@ -1221,31 +1300,31 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="4" t="n"/>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="I23" s="35" t="s">
+      <c r="I23" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K23" s="35" t="n">
+      <c r="K23" s="44" t="n">
         <v>3</v>
       </c>
       <c r="M23" s="10" t="n"/>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="4" t="n"/>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="36" t="n"/>
-      <c r="K24" s="36" t="n"/>
-      <c r="M24" s="35" t="n">
+      <c r="I24" s="48" t="n"/>
+      <c r="K24" s="48" t="n"/>
+      <c r="M24" s="44" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1256,77 +1335,85 @@
       <c r="A26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="34" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="4" t="n"/>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="31" t="s">
+      <c r="G27" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="I27" s="35" t="n"/>
-      <c r="K27" s="35" t="n"/>
+      <c r="I27" s="44" t="n"/>
+      <c r="K27" s="44" t="n"/>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="4" t="n"/>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="31" t="s">
+      <c r="G28" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="I28" s="36" t="n"/>
-      <c r="K28" s="36" t="n"/>
+      <c r="I28" s="48" t="n"/>
+      <c r="K28" s="48" t="n"/>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="4" t="n"/>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="G29" s="31" t="s">
+      <c r="G29" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="I29" s="36" t="n"/>
-      <c r="K29" s="36" t="n"/>
+      <c r="I29" s="48" t="n"/>
+      <c r="K29" s="48" t="n"/>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="4" t="n"/>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="31" t="n"/>
-      <c r="I30" s="36" t="n"/>
+      <c r="G30" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="I30" s="48" t="s">
+        <v>27</v>
+      </c>
       <c r="J30" s="10" t="n"/>
-      <c r="K30" s="36" t="n"/>
+      <c r="K30" s="48" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="4" t="n"/>
-      <c r="B31" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>27</v>
-      </c>
+      <c r="B31" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="I31" s="10" t="n"/>
       <c r="J31" s="10" t="n"/>
-      <c r="K31" s="10" t="n">
-        <v>4</v>
-      </c>
+      <c r="K31" s="10" t="n"/>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="4" t="n"/>
-      <c r="B32" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="G32" s="31" t="n"/>
-      <c r="I32" s="35" t="n"/>
+      <c r="B32" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="I32" s="44" t="s">
+        <v>27</v>
+      </c>
       <c r="J32" s="10" t="n"/>
-      <c r="K32" s="35" t="n"/>
-      <c r="M32" s="35" t="n">
-        <v>8</v>
+      <c r="K32" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="M32" s="44" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -1337,26 +1424,26 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="38" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="4" t="n"/>
-      <c r="B35" s="31" t="n"/>
-      <c r="G35" s="31" t="n"/>
-      <c r="I35" s="35" t="n"/>
-      <c r="K35" s="35" t="n"/>
+      <c r="B35" s="32" t="n"/>
+      <c r="G35" s="32" t="n"/>
+      <c r="I35" s="44" t="n"/>
+      <c r="K35" s="44" t="n"/>
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="4" t="n"/>
-      <c r="B36" s="31" t="n"/>
-      <c r="G36" s="31" t="n"/>
-      <c r="I36" s="36" t="n"/>
-      <c r="K36" s="36" t="n"/>
-      <c r="M36" s="35" t="n">
+      <c r="B36" s="32" t="n"/>
+      <c r="G36" s="32" t="n"/>
+      <c r="I36" s="48" t="n"/>
+      <c r="K36" s="48" t="n"/>
+      <c r="M36" s="44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1368,16 +1455,16 @@
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" s="38" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="4" t="n"/>
-      <c r="B39" s="31" t="s">
-        <v>64</v>
+      <c r="B39" s="32" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -1385,476 +1472,476 @@
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="4" t="n"/>
-      <c r="B41" s="33" t="s">
-        <v>65</v>
+      <c r="B41" s="37" t="s">
+        <v>67</v>
       </c>
       <c r="I41" s="10" t="n"/>
       <c r="K41" s="10" t="n"/>
     </row>
     <row r="42" spans="1:14">
       <c r="A42" s="4" t="n"/>
-      <c r="B42" s="33" t="s">
-        <v>66</v>
+      <c r="B42" s="37" t="s">
+        <v>68</v>
       </c>
       <c r="I42" s="10" t="n"/>
       <c r="K42" s="10" t="n"/>
     </row>
     <row r="43" spans="1:14">
       <c r="A43" s="4" t="n"/>
-      <c r="B43" s="33" t="s">
-        <v>67</v>
+      <c r="B43" s="37" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:14">
       <c r="A44" s="4" t="n"/>
-      <c r="B44" s="33" t="s">
-        <v>68</v>
+      <c r="B44" s="37" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="4" t="n"/>
-      <c r="B45" s="33" t="s">
-        <v>69</v>
+      <c r="B45" s="37" t="s">
+        <v>71</v>
       </c>
       <c r="I45" s="10" t="n"/>
       <c r="K45" s="10" t="n"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="4" t="n"/>
-      <c r="B46" s="33" t="s">
-        <v>70</v>
+      <c r="B46" s="37" t="s">
+        <v>72</v>
       </c>
       <c r="I46" s="10" t="n"/>
       <c r="K46" s="10" t="n"/>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="4" t="n"/>
-      <c r="B47" s="33" t="s">
-        <v>71</v>
+      <c r="B47" s="37" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="4" t="n"/>
-      <c r="B48" s="31" t="n"/>
-      <c r="G48" s="31" t="n"/>
+      <c r="B48" s="32" t="n"/>
+      <c r="G48" s="32" t="n"/>
       <c r="I48" s="10" t="n"/>
       <c r="K48" s="10" t="n"/>
     </row>
     <row r="49" spans="1:14">
       <c r="A49" s="4" t="n"/>
-      <c r="B49" s="34" t="n"/>
-      <c r="F49" s="35" t="n"/>
-      <c r="H49" s="35" t="n"/>
-      <c r="I49" s="35" t="n"/>
-      <c r="K49" s="35" t="n"/>
+      <c r="B49" s="46" t="n"/>
+      <c r="F49" s="44" t="n"/>
+      <c r="H49" s="44" t="n"/>
+      <c r="I49" s="44" t="n"/>
+      <c r="K49" s="44" t="n"/>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" s="4" t="n"/>
-      <c r="B50" s="34" t="n"/>
-      <c r="F50" s="36" t="n"/>
-      <c r="H50" s="35" t="n"/>
-      <c r="I50" s="36" t="n"/>
-      <c r="K50" s="36" t="n"/>
+      <c r="B50" s="46" t="n"/>
+      <c r="F50" s="48" t="n"/>
+      <c r="H50" s="44" t="n"/>
+      <c r="I50" s="48" t="n"/>
+      <c r="K50" s="48" t="n"/>
     </row>
     <row r="51" spans="1:14">
       <c r="A51" s="4" t="n"/>
-      <c r="B51" s="34" t="n"/>
-      <c r="F51" s="36" t="n"/>
-      <c r="H51" s="35" t="n"/>
-      <c r="I51" s="36" t="n"/>
-      <c r="K51" s="36" t="n"/>
+      <c r="B51" s="46" t="n"/>
+      <c r="F51" s="48" t="n"/>
+      <c r="H51" s="44" t="n"/>
+      <c r="I51" s="48" t="n"/>
+      <c r="K51" s="48" t="n"/>
     </row>
     <row r="52" spans="1:14">
       <c r="A52" s="4" t="n"/>
-      <c r="B52" s="34" t="n"/>
-      <c r="F52" s="36" t="n"/>
-      <c r="H52" s="35" t="n"/>
-      <c r="I52" s="35" t="n"/>
-      <c r="K52" s="35" t="n"/>
+      <c r="B52" s="46" t="n"/>
+      <c r="F52" s="48" t="n"/>
+      <c r="H52" s="44" t="n"/>
+      <c r="I52" s="44" t="n"/>
+      <c r="K52" s="44" t="n"/>
     </row>
     <row r="53" spans="1:14">
       <c r="A53" s="4" t="n"/>
-      <c r="B53" s="34" t="n"/>
-      <c r="F53" s="36" t="n"/>
-      <c r="H53" s="35" t="n"/>
-      <c r="I53" s="35" t="n"/>
-      <c r="K53" s="35" t="n"/>
+      <c r="B53" s="46" t="n"/>
+      <c r="F53" s="48" t="n"/>
+      <c r="H53" s="44" t="n"/>
+      <c r="I53" s="44" t="n"/>
+      <c r="K53" s="44" t="n"/>
       <c r="M53" s="10" t="n"/>
     </row>
     <row r="54" spans="1:14">
       <c r="A54" s="4" t="n"/>
-      <c r="B54" s="34" t="n"/>
-      <c r="F54" s="36" t="n"/>
-      <c r="H54" s="35" t="n"/>
-      <c r="I54" s="36" t="n"/>
-      <c r="K54" s="36" t="n"/>
+      <c r="B54" s="46" t="n"/>
+      <c r="F54" s="48" t="n"/>
+      <c r="H54" s="44" t="n"/>
+      <c r="I54" s="48" t="n"/>
+      <c r="K54" s="48" t="n"/>
       <c r="M54" s="10" t="n"/>
     </row>
     <row r="55" spans="1:14">
       <c r="A55" s="4" t="n"/>
-      <c r="B55" s="33" t="n"/>
-      <c r="G55" s="33" t="n"/>
+      <c r="B55" s="37" t="n"/>
+      <c r="G55" s="37" t="n"/>
       <c r="I55" s="10" t="n"/>
       <c r="K55" s="10" t="n"/>
       <c r="M55" s="10" t="n"/>
     </row>
     <row r="56" spans="1:14">
       <c r="A56" s="4" t="n"/>
-      <c r="B56" s="33" t="n"/>
+      <c r="B56" s="37" t="n"/>
       <c r="I56" s="10" t="n"/>
       <c r="K56" s="10" t="n"/>
       <c r="M56" s="10" t="n"/>
     </row>
     <row r="57" spans="1:14">
       <c r="A57" s="4" t="n"/>
-      <c r="B57" s="33" t="n"/>
-      <c r="C57" s="33" t="n"/>
-      <c r="D57" s="33" t="n"/>
-      <c r="E57" s="33" t="n"/>
-      <c r="F57" s="33" t="n"/>
-      <c r="G57" s="33" t="n"/>
-      <c r="H57" s="33" t="n"/>
+      <c r="B57" s="37" t="n"/>
+      <c r="C57" s="37" t="n"/>
+      <c r="D57" s="37" t="n"/>
+      <c r="E57" s="37" t="n"/>
+      <c r="F57" s="37" t="n"/>
+      <c r="G57" s="37" t="n"/>
+      <c r="H57" s="37" t="n"/>
       <c r="I57" s="10" t="n"/>
       <c r="K57" s="10" t="n"/>
-      <c r="M57" s="35" t="n">
+      <c r="M57" s="44" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:14">
       <c r="A58" s="4" t="n"/>
-      <c r="B58" s="33" t="n"/>
-      <c r="C58" s="33" t="n"/>
-      <c r="D58" s="33" t="n"/>
-      <c r="E58" s="33" t="n"/>
-      <c r="F58" s="33" t="n"/>
-      <c r="G58" s="33" t="n"/>
-      <c r="H58" s="33" t="n"/>
+      <c r="B58" s="37" t="n"/>
+      <c r="C58" s="37" t="n"/>
+      <c r="D58" s="37" t="n"/>
+      <c r="E58" s="37" t="n"/>
+      <c r="F58" s="37" t="n"/>
+      <c r="G58" s="37" t="n"/>
+      <c r="H58" s="37" t="n"/>
       <c r="I58" s="10" t="n"/>
       <c r="K58" s="10" t="n"/>
       <c r="M58" s="10" t="n"/>
     </row>
     <row r="59" spans="1:14">
       <c r="A59" s="4" t="n"/>
-      <c r="B59" s="33" t="n"/>
-      <c r="C59" s="33" t="n"/>
-      <c r="D59" s="33" t="n"/>
-      <c r="E59" s="33" t="n"/>
-      <c r="F59" s="33" t="n"/>
-      <c r="G59" s="33" t="n"/>
-      <c r="H59" s="33" t="n"/>
+      <c r="B59" s="37" t="n"/>
+      <c r="C59" s="37" t="n"/>
+      <c r="D59" s="37" t="n"/>
+      <c r="E59" s="37" t="n"/>
+      <c r="F59" s="37" t="n"/>
+      <c r="G59" s="37" t="n"/>
+      <c r="H59" s="37" t="n"/>
       <c r="I59" s="10" t="n"/>
       <c r="K59" s="10" t="n"/>
       <c r="M59" s="10" t="n"/>
     </row>
     <row r="60" spans="1:14">
       <c r="A60" s="4" t="n"/>
-      <c r="B60" s="33" t="n"/>
-      <c r="F60" s="33" t="n"/>
-      <c r="G60" s="33" t="n"/>
+      <c r="B60" s="37" t="n"/>
+      <c r="F60" s="37" t="n"/>
+      <c r="G60" s="37" t="n"/>
       <c r="I60" s="10" t="n"/>
       <c r="K60" s="10" t="n"/>
     </row>
     <row r="61" spans="1:14">
       <c r="A61" s="4" t="n"/>
-      <c r="B61" s="33" t="n"/>
-      <c r="C61" s="33" t="n"/>
-      <c r="D61" s="33" t="n"/>
-      <c r="E61" s="33" t="n"/>
-      <c r="F61" s="33" t="n"/>
-      <c r="G61" s="33" t="n"/>
-      <c r="H61" s="33" t="n"/>
+      <c r="B61" s="37" t="n"/>
+      <c r="C61" s="37" t="n"/>
+      <c r="D61" s="37" t="n"/>
+      <c r="E61" s="37" t="n"/>
+      <c r="F61" s="37" t="n"/>
+      <c r="G61" s="37" t="n"/>
+      <c r="H61" s="37" t="n"/>
       <c r="I61" s="10" t="n"/>
       <c r="K61" s="10" t="n"/>
     </row>
     <row r="62" spans="1:14">
       <c r="A62" s="4" t="n"/>
-      <c r="I62" s="40" t="s">
+      <c r="I62" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="J62" s="40" t="n">
+      <c r="J62" s="43" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:14">
       <c r="A63" s="4" t="n"/>
-      <c r="I63" s="40" t="n"/>
-      <c r="J63" s="40" t="n"/>
-      <c r="K63" s="40" t="n"/>
-      <c r="L63" s="40" t="n"/>
-      <c r="M63" s="40" t="n"/>
+      <c r="I63" s="43" t="n"/>
+      <c r="J63" s="43" t="n"/>
+      <c r="K63" s="43" t="n"/>
+      <c r="L63" s="43" t="n"/>
+      <c r="M63" s="43" t="n"/>
     </row>
     <row r="64" spans="1:14">
       <c r="A64" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B64" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="B64" s="34" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:14">
       <c r="A65" s="4" t="n"/>
-      <c r="B65" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="G65" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="I65" s="35" t="s">
+      <c r="B65" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="G65" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="I65" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K65" s="35" t="n">
+      <c r="K65" s="44" t="n">
         <v>3</v>
       </c>
-      <c r="M65" s="35" t="n">
+      <c r="M65" s="44" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:14">
       <c r="A66" s="4" t="n"/>
-      <c r="G66" s="32" t="n"/>
+      <c r="G66" s="39" t="n"/>
       <c r="I66" s="13" t="n"/>
       <c r="K66" s="13" t="n"/>
     </row>
     <row r="67" spans="1:14">
       <c r="A67" s="4" t="n"/>
-      <c r="I67" s="40" t="n"/>
-      <c r="J67" s="40" t="n"/>
-      <c r="K67" s="40" t="n"/>
-      <c r="L67" s="40" t="n"/>
-      <c r="M67" s="40" t="n"/>
+      <c r="I67" s="43" t="n"/>
+      <c r="J67" s="43" t="n"/>
+      <c r="K67" s="43" t="n"/>
+      <c r="L67" s="43" t="n"/>
+      <c r="M67" s="43" t="n"/>
     </row>
     <row r="68" spans="1:14">
       <c r="A68" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B68" s="38" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="B68" s="34" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:14">
       <c r="A69" s="4" t="n"/>
-      <c r="B69" s="37" t="s">
-        <v>78</v>
+      <c r="B69" s="47" t="s">
+        <v>80</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="70" spans="1:14">
       <c r="A70" s="4" t="n"/>
-      <c r="B70" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="G70" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="I70" s="35" t="n"/>
-      <c r="K70" s="35" t="n"/>
+      <c r="B70" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="G70" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="I70" s="44" t="n"/>
+      <c r="K70" s="44" t="n"/>
     </row>
     <row r="71" spans="1:14">
       <c r="A71" s="4" t="n"/>
-      <c r="B71" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="G71" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="I71" s="36" t="n"/>
-      <c r="K71" s="36" t="n"/>
+      <c r="B71" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="G71" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="I71" s="48" t="n"/>
+      <c r="K71" s="48" t="n"/>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="31" t="n"/>
-      <c r="B72" s="37" t="s">
-        <v>83</v>
+      <c r="A72" s="32" t="n"/>
+      <c r="B72" s="47" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:14">
       <c r="A73" s="4" t="n"/>
-      <c r="B73" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="G73" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="I73" s="35" t="n"/>
-      <c r="K73" s="35" t="n"/>
+      <c r="B73" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="G73" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="I73" s="44" t="n"/>
+      <c r="K73" s="44" t="n"/>
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="4" t="n"/>
-      <c r="B74" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="G74" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="I74" s="35" t="n"/>
-      <c r="K74" s="35" t="n"/>
+      <c r="B74" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G74" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="I74" s="44" t="n"/>
+      <c r="K74" s="44" t="n"/>
     </row>
     <row r="75" spans="1:14">
       <c r="A75" s="4" t="n"/>
-      <c r="G75" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="I75" s="35" t="n"/>
-      <c r="K75" s="35" t="n"/>
+      <c r="G75" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="I75" s="44" t="n"/>
+      <c r="K75" s="44" t="n"/>
     </row>
     <row customHeight="1" ht="13.5" r="76" spans="1:14">
       <c r="A76" s="4" t="n"/>
-      <c r="B76" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="G76" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="I76" s="36" t="n"/>
+      <c r="B76" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G76" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="I76" s="48" t="n"/>
       <c r="J76" s="10" t="n"/>
-      <c r="K76" s="36" t="n"/>
+      <c r="K76" s="48" t="n"/>
     </row>
     <row r="77" spans="1:14">
       <c r="A77" s="4" t="n"/>
-      <c r="B77" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="G77" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="I77" s="35" t="n"/>
+      <c r="B77" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="G77" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="I77" s="44" t="n"/>
       <c r="J77" s="10" t="n"/>
-      <c r="K77" s="35" t="n"/>
+      <c r="K77" s="44" t="n"/>
     </row>
     <row r="78" spans="1:14">
       <c r="A78" s="4" t="n"/>
-      <c r="B78" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="D78" s="33" t="n"/>
-      <c r="E78" s="33" t="n"/>
-      <c r="F78" s="33" t="n"/>
-      <c r="G78" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="I78" s="35" t="n"/>
+      <c r="B78" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D78" s="37" t="n"/>
+      <c r="E78" s="37" t="n"/>
+      <c r="F78" s="37" t="n"/>
+      <c r="G78" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="I78" s="44" t="n"/>
       <c r="J78" s="10" t="n"/>
-      <c r="K78" s="35" t="n"/>
+      <c r="K78" s="44" t="n"/>
     </row>
     <row r="79" spans="1:14">
       <c r="A79" s="4" t="n"/>
-      <c r="B79" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="G79" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="I79" s="35" t="n"/>
-      <c r="K79" s="35" t="n"/>
+      <c r="B79" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="G79" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="I79" s="44" t="n"/>
+      <c r="K79" s="44" t="n"/>
     </row>
     <row r="80" spans="1:14">
       <c r="A80" s="4" t="n"/>
-      <c r="B80" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="G80" s="31" t="s">
-        <v>98</v>
+      <c r="B80" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="G80" s="32" t="s">
+        <v>100</v>
       </c>
       <c r="I80" s="10" t="n"/>
       <c r="K80" s="10" t="n"/>
     </row>
     <row r="81" spans="1:14">
       <c r="A81" s="4" t="n"/>
-      <c r="B81" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="G81" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="I81" s="36" t="n"/>
-      <c r="K81" s="36" t="n"/>
+      <c r="B81" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="G81" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="I81" s="48" t="n"/>
+      <c r="K81" s="48" t="n"/>
     </row>
     <row r="82" spans="1:14">
       <c r="A82" s="4" t="n"/>
       <c r="B82" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="I82" s="40" t="n"/>
-      <c r="J82" s="40" t="n"/>
-      <c r="K82" s="40" t="n"/>
-      <c r="L82" s="40" t="n"/>
-      <c r="M82" s="40" t="n"/>
+        <v>103</v>
+      </c>
+      <c r="I82" s="43" t="n"/>
+      <c r="J82" s="43" t="n"/>
+      <c r="K82" s="43" t="n"/>
+      <c r="L82" s="43" t="n"/>
+      <c r="M82" s="43" t="n"/>
     </row>
     <row r="83" spans="1:14">
       <c r="A83" s="4" t="n"/>
-      <c r="B83" s="31" t="s">
-        <v>102</v>
+      <c r="B83" s="32" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:14">
       <c r="A84" s="4" t="n"/>
-      <c r="B84" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="G84" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="I84" s="35" t="s">
+      <c r="B84" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G84" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="I84" s="44" t="s">
         <v>27</v>
       </c>
       <c r="J84" s="10" t="n"/>
-      <c r="K84" s="35" t="n">
+      <c r="K84" s="44" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:14">
       <c r="A85" s="4" t="n"/>
-      <c r="B85" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="G85" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="I85" s="35" t="s">
+      <c r="B85" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="G85" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="I85" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="K85" s="35" t="n">
+      <c r="K85" s="44" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:14">
       <c r="A86" s="4" t="n"/>
-      <c r="B86" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="G86" s="31" t="n"/>
-      <c r="I86" s="35" t="n"/>
-      <c r="K86" s="35" t="n"/>
+      <c r="B86" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G86" s="32" t="n"/>
+      <c r="I86" s="44" t="n"/>
+      <c r="K86" s="44" t="n"/>
     </row>
     <row r="87" spans="1:14">
       <c r="A87" s="4" t="n"/>
-      <c r="B87" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="I87" s="36" t="n"/>
-      <c r="K87" s="36" t="n"/>
+      <c r="B87" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="I87" s="48" t="n"/>
+      <c r="K87" s="48" t="n"/>
     </row>
     <row r="88" spans="1:14">
       <c r="A88" s="4" t="n"/>
-      <c r="B88" s="31" t="s">
-        <v>109</v>
+      <c r="B88" s="32" t="s">
+        <v>111</v>
       </c>
       <c r="I88" s="10" t="n"/>
       <c r="K88" s="10" t="n"/>
     </row>
     <row r="89" spans="1:14">
       <c r="A89" s="4" t="n"/>
-      <c r="B89" s="31" t="n"/>
-      <c r="G89" s="31" t="n"/>
-      <c r="I89" s="36" t="n"/>
-      <c r="K89" s="36" t="n"/>
+      <c r="B89" s="32" t="n"/>
+      <c r="G89" s="32" t="n"/>
+      <c r="I89" s="48" t="n"/>
+      <c r="K89" s="48" t="n"/>
     </row>
     <row r="90" spans="1:14">
       <c r="A90" s="4" t="n"/>
-      <c r="B90" s="31" t="n"/>
-      <c r="G90" s="31" t="n"/>
-      <c r="I90" s="36" t="n"/>
-      <c r="K90" s="36" t="n"/>
-      <c r="M90" s="35" t="n">
-        <v>10</v>
+      <c r="B90" s="32" t="n"/>
+      <c r="G90" s="32" t="n"/>
+      <c r="I90" s="48" t="n"/>
+      <c r="K90" s="48" t="n"/>
+      <c r="M90" s="44" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:14">
@@ -1862,33 +1949,33 @@
     </row>
     <row r="92" spans="1:14">
       <c r="A92" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B92" s="38" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="B92" s="34" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="93" spans="1:14">
       <c r="A93" s="4" t="n"/>
-      <c r="B93" s="31" t="n"/>
-      <c r="G93" s="41" t="n"/>
-      <c r="I93" s="35" t="n"/>
-      <c r="K93" s="35" t="n"/>
+      <c r="B93" s="32" t="n"/>
+      <c r="G93" s="45" t="n"/>
+      <c r="I93" s="44" t="n"/>
+      <c r="K93" s="44" t="n"/>
     </row>
     <row r="94" spans="1:14">
       <c r="A94" s="4" t="n"/>
-      <c r="B94" s="31" t="n"/>
-      <c r="G94" s="31" t="n"/>
-      <c r="I94" s="35" t="n"/>
-      <c r="K94" s="35" t="n"/>
+      <c r="B94" s="32" t="n"/>
+      <c r="G94" s="32" t="n"/>
+      <c r="I94" s="44" t="n"/>
+      <c r="K94" s="44" t="n"/>
     </row>
     <row r="95" spans="1:14">
       <c r="A95" s="4" t="n"/>
-      <c r="B95" s="31" t="n"/>
-      <c r="G95" s="31" t="n"/>
-      <c r="I95" s="36" t="n"/>
-      <c r="K95" s="36" t="n"/>
-      <c r="M95" s="35" t="n">
+      <c r="B95" s="32" t="n"/>
+      <c r="G95" s="32" t="n"/>
+      <c r="I95" s="48" t="n"/>
+      <c r="K95" s="48" t="n"/>
+      <c r="M95" s="44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1900,75 +1987,75 @@
     </row>
     <row r="97" spans="1:14">
       <c r="A97" s="4" t="n"/>
-      <c r="B97" s="31" t="n"/>
+      <c r="B97" s="32" t="n"/>
     </row>
     <row r="98" spans="1:14">
       <c r="A98" s="4" t="n"/>
       <c r="I98" s="10" t="n"/>
-      <c r="J98" s="44" t="s">
-        <v>112</v>
+      <c r="J98" s="31" t="s">
+        <v>114</v>
       </c>
       <c r="K98" s="10" t="n"/>
       <c r="L98" s="10" t="n"/>
-      <c r="M98" s="35" t="n">
-        <v>29</v>
+      <c r="M98" s="44" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="99" spans="1:14">
       <c r="A99" s="4" t="n"/>
-      <c r="J99" s="47" t="n"/>
-      <c r="K99" s="39" t="n"/>
-      <c r="L99" s="39" t="s">
-        <v>113</v>
+      <c r="J99" s="36" t="n"/>
+      <c r="K99" s="42" t="n"/>
+      <c r="L99" s="42" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="100" spans="1:14">
       <c r="A100" s="4" t="n"/>
-      <c r="B100" s="35" t="n"/>
-      <c r="C100" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="H100" s="35" t="n"/>
+      <c r="B100" s="44" t="n"/>
+      <c r="C100" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="H100" s="44" t="n"/>
     </row>
     <row r="101" spans="1:14">
       <c r="A101" s="4" t="n"/>
-      <c r="B101" s="36" t="n"/>
-      <c r="C101" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="H101" s="35" t="n"/>
+      <c r="B101" s="48" t="n"/>
+      <c r="C101" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="H101" s="44" t="n"/>
     </row>
     <row r="102" spans="1:14">
       <c r="A102" s="4" t="n"/>
-      <c r="B102" s="36" t="n"/>
-      <c r="C102" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="H102" s="35" t="n"/>
+      <c r="B102" s="48" t="n"/>
+      <c r="C102" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="H102" s="44" t="n"/>
     </row>
     <row r="103" spans="1:14">
       <c r="A103" s="4" t="n"/>
     </row>
     <row r="104" spans="1:14">
       <c r="A104" s="4" t="n"/>
-      <c r="B104" s="35" t="n"/>
-      <c r="C104" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="G104" s="34" t="n"/>
-      <c r="H104" s="31" t="s">
-        <v>118</v>
+      <c r="B104" s="44" t="n"/>
+      <c r="C104" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="G104" s="46" t="n"/>
+      <c r="H104" s="32" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="105" spans="1:14">
       <c r="A105" s="4" t="n"/>
-      <c r="B105" s="36" t="n"/>
-      <c r="C105" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="G105" s="34" t="n"/>
-      <c r="H105" s="31" t="s">
+      <c r="B105" s="48" t="n"/>
+      <c r="C105" s="32" t="s">
         <v>119</v>
+      </c>
+      <c r="G105" s="46" t="n"/>
+      <c r="H105" s="32" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="106" spans="1:14">
@@ -1978,64 +2065,294 @@
     <row r="107" spans="1:14">
       <c r="A107" s="4" t="n"/>
       <c r="B107" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C107" s="32" t="n"/>
-      <c r="D107" s="32" t="n"/>
-      <c r="E107" s="32" t="n"/>
-      <c r="F107" s="32" t="n"/>
-      <c r="G107" s="32" t="n"/>
-      <c r="H107" s="32" t="n"/>
-      <c r="I107" s="32" t="n"/>
-      <c r="J107" s="32" t="n"/>
-      <c r="K107" s="32" t="n"/>
+        <v>122</v>
+      </c>
+      <c r="C107" s="39" t="n"/>
+      <c r="D107" s="39" t="n"/>
+      <c r="E107" s="39" t="n"/>
+      <c r="F107" s="39" t="n"/>
+      <c r="G107" s="39" t="n"/>
+      <c r="H107" s="39" t="n"/>
+      <c r="I107" s="39" t="n"/>
+      <c r="J107" s="39" t="n"/>
+      <c r="K107" s="39" t="n"/>
     </row>
     <row r="108" spans="1:14">
       <c r="A108" s="4" t="n"/>
       <c r="B108" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C108" s="32" t="n"/>
-      <c r="D108" s="32" t="n"/>
-      <c r="E108" s="32" t="n"/>
-      <c r="F108" s="32" t="n"/>
-      <c r="G108" s="32" t="n"/>
-      <c r="H108" s="32" t="n"/>
-      <c r="I108" s="32" t="n"/>
-      <c r="J108" s="32" t="n"/>
-      <c r="K108" s="32" t="n"/>
+        <v>123</v>
+      </c>
+      <c r="C108" s="39" t="n"/>
+      <c r="D108" s="39" t="n"/>
+      <c r="E108" s="39" t="n"/>
+      <c r="F108" s="39" t="n"/>
+      <c r="G108" s="39" t="n"/>
+      <c r="H108" s="39" t="n"/>
+      <c r="I108" s="39" t="n"/>
+      <c r="J108" s="39" t="n"/>
+      <c r="K108" s="39" t="n"/>
     </row>
     <row r="109" spans="1:14">
       <c r="A109" s="4" t="n"/>
       <c r="B109" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C109" s="32" t="n"/>
-      <c r="D109" s="32" t="n"/>
-      <c r="E109" s="32" t="n"/>
-      <c r="F109" s="32" t="n"/>
-      <c r="G109" s="32" t="n"/>
-      <c r="H109" s="32" t="n"/>
-      <c r="I109" s="32" t="n"/>
-      <c r="J109" s="32" t="n"/>
-      <c r="K109" s="32" t="n"/>
+        <v>124</v>
+      </c>
+      <c r="C109" s="39" t="n"/>
+      <c r="D109" s="39" t="n"/>
+      <c r="E109" s="39" t="n"/>
+      <c r="F109" s="39" t="n"/>
+      <c r="G109" s="39" t="n"/>
+      <c r="H109" s="39" t="n"/>
+      <c r="I109" s="39" t="n"/>
+      <c r="J109" s="39" t="n"/>
+      <c r="K109" s="39" t="n"/>
     </row>
     <row r="110" spans="1:14">
       <c r="A110" s="4" t="n"/>
-      <c r="C110" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="H110" s="38" t="n"/>
-      <c r="K110" s="38" t="s">
-        <v>124</v>
+      <c r="C110" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="H110" s="34" t="n"/>
+      <c r="K110" s="34" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="111" spans="1:14">
-      <c r="E111" s="38" t="n"/>
-      <c r="H111" s="38" t="n"/>
+      <c r="E111" s="34" t="n"/>
+      <c r="H111" s="34" t="n"/>
+      <c r="K111" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14">
+      <c r="K112" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14">
+      <c r="K113" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14">
+      <c r="K114" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14">
+      <c r="K115" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14">
+      <c r="K116" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14">
+      <c r="K117" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14">
+      <c r="K118" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14">
+      <c r="K119" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14">
+      <c r="K120" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14">
+      <c r="K121" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14">
+      <c r="K122" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14">
+      <c r="K123" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14">
+      <c r="K124" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14">
+      <c r="K125" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14">
+      <c r="K126" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14">
+      <c r="K127" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14">
+      <c r="K128" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14">
+      <c r="K129" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14">
+      <c r="K130" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14">
+      <c r="K131" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14">
+      <c r="K132" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14">
+      <c r="K133" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14">
+      <c r="K134" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14">
+      <c r="K135" t="s">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="131">
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="B83:K83"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="B72:H72"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="C104:F104"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="G84:H84"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="B38:M38"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="G95:H95"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B56:H56"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="B87:E87"/>
+    <mergeCell ref="L99:M99"/>
+    <mergeCell ref="B97:K97"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="B84:E84"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B92:E92"/>
+    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B88:E88"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G29:H29"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -2060,113 +2377,6 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="J7:L7"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="L99:M99"/>
-    <mergeCell ref="B97:K97"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="B84:E84"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B92:E92"/>
-    <mergeCell ref="G93:H93"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="G90:H90"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B88:E88"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="B38:M38"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="G95:H95"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="G80:H80"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B56:H56"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="G94:H94"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="B87:E87"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="C104:F104"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="B83:K83"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="B72:H72"/>
   </mergeCells>
   <pageMargins bottom="0.5" footer="0.5" header="0.5" left="0.25" right="0.25" top="0.5"/>
   <pageSetup horizontalDpi="4294967292" orientation="portrait" scale="95"/>

</xml_diff>